<commit_message>
add html supporting files if not exist
</commit_message>
<xml_diff>
--- a/OfficeReport.xlsx
+++ b/OfficeReport.xlsx
@@ -237,7 +237,7 @@
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="1154861883" name="Picture">
+        <xdr:cNvPr id="412047054" name="Picture">
 </xdr:cNvPr>
         <xdr:cNvPicPr/>
       </xdr:nvPicPr>
@@ -493,7 +493,7 @@
       <c r="J7" s="4" t="inlineStr">
         <is>
           <r>
-            <t xml:space="preserve">2024-11-04 - 2024-11-05</t>
+            <t xml:space="preserve">2024-11-01 - 2024-11-08</t>
           </r>
         </is>
       </c>
@@ -522,7 +522,7 @@
       <c r="E8" s="5" t="inlineStr">
         <is>
           <r>
-            <t xml:space="preserve">2024-11-05T19:53:</t>
+            <t xml:space="preserve">2024-11-08T14:58:</t>
           </r>
         </is>
       </c>
@@ -792,7 +792,7 @@
       <c r="C16" s="9" t="inlineStr">
         <is>
           <r>
-            <t xml:space="preserve">SP</t>
+            <t xml:space="preserve">USD</t>
           </r>
         </is>
       </c>
@@ -802,7 +802,7 @@
       <c r="G16" s="9" t="inlineStr">
         <is>
           <r>
-            <t xml:space="preserve">4000000.0</t>
+            <t xml:space="preserve">4800000.0</t>
           </r>
         </is>
       </c>
@@ -815,7 +815,7 @@
       <c r="N16" s="9" t="inlineStr">
         <is>
           <r>
-            <t xml:space="preserve">1</t>
+            <t xml:space="preserve">2</t>
           </r>
         </is>
       </c>
@@ -884,7 +884,7 @@
       <c r="C18" s="9" t="inlineStr">
         <is>
           <r>
-            <t xml:space="preserve">USD</t>
+            <t xml:space="preserve">SP</t>
           </r>
         </is>
       </c>
@@ -894,7 +894,7 @@
       <c r="G18" s="9" t="inlineStr">
         <is>
           <r>
-            <t xml:space="preserve">800000.0</t>
+            <t xml:space="preserve">4000000.0</t>
           </r>
         </is>
       </c>
@@ -915,7 +915,7 @@
       <c r="P18" s="9" t="inlineStr">
         <is>
           <r>
-            <t xml:space="preserve">هوزان يوسف يوسف </t>
+            <t xml:space="preserve">عبد الجواد اللايح</t>
           </r>
         </is>
       </c>
@@ -926,7 +926,7 @@
       <c r="U18" s="9" t="inlineStr">
         <is>
           <r>
-            <t xml:space="preserve">250629</t>
+            <t xml:space="preserve">251716</t>
           </r>
         </is>
       </c>
@@ -935,7 +935,7 @@
       <c r="X18" s="10" t="inlineStr">
         <is>
           <r>
-            <t xml:space="preserve">35</t>
+            <t xml:space="preserve">339</t>
           </r>
         </is>
       </c>
@@ -976,7 +976,7 @@
       <c r="C20" s="9" t="inlineStr">
         <is>
           <r>
-            <t xml:space="preserve">SP</t>
+            <t xml:space="preserve">USD</t>
           </r>
         </is>
       </c>
@@ -986,7 +986,7 @@
       <c r="G20" s="9" t="inlineStr">
         <is>
           <r>
-            <t xml:space="preserve">4000000.0</t>
+            <t xml:space="preserve">880000.0</t>
           </r>
         </is>
       </c>
@@ -1007,7 +1007,7 @@
       <c r="P20" s="9" t="inlineStr">
         <is>
           <r>
-            <t xml:space="preserve">عبد الجواد اللايح</t>
+            <t xml:space="preserve">عاصم شيخو</t>
           </r>
         </is>
       </c>
@@ -1018,7 +1018,7 @@
       <c r="U20" s="9" t="inlineStr">
         <is>
           <r>
-            <t xml:space="preserve">251716</t>
+            <t xml:space="preserve">829983</t>
           </r>
         </is>
       </c>
@@ -1027,14 +1027,14 @@
       <c r="X20" s="10" t="inlineStr">
         <is>
           <r>
-            <t xml:space="preserve">339</t>
+            <t xml:space="preserve">51</t>
           </r>
         </is>
       </c>
       <c r="Y20" s="1" t="inlineStr"/>
       <c r="Z20" s="1" t="inlineStr"/>
     </row>
-    <row r="21" customHeight="1" ht="6">
+    <row r="21" customHeight="1" ht="802">
       <c r="A21" s="1" t="inlineStr"/>
       <c r="B21" s="1" t="inlineStr"/>
       <c r="C21" s="1" t="inlineStr"/>
@@ -1062,98 +1062,6 @@
       <c r="Y21" s="1" t="inlineStr"/>
       <c r="Z21" s="1" t="inlineStr"/>
     </row>
-    <row r="22" customHeight="1" ht="30">
-      <c r="A22" s="1" t="inlineStr"/>
-      <c r="B22" s="1" t="inlineStr"/>
-      <c r="C22" s="9" t="inlineStr">
-        <is>
-          <r>
-            <t xml:space="preserve">USD</t>
-          </r>
-        </is>
-      </c>
-      <c r="D22" s="9" t="inlineStr"/>
-      <c r="E22" s="9" t="inlineStr"/>
-      <c r="F22" s="1" t="inlineStr"/>
-      <c r="G22" s="9" t="inlineStr">
-        <is>
-          <r>
-            <t xml:space="preserve">880000.0</t>
-          </r>
-        </is>
-      </c>
-      <c r="H22" s="9" t="inlineStr"/>
-      <c r="I22" s="9" t="inlineStr"/>
-      <c r="J22" s="9" t="inlineStr"/>
-      <c r="K22" s="9" t="inlineStr"/>
-      <c r="L22" s="9" t="inlineStr"/>
-      <c r="M22" s="1" t="inlineStr"/>
-      <c r="N22" s="9" t="inlineStr">
-        <is>
-          <r>
-            <t xml:space="preserve">1</t>
-          </r>
-        </is>
-      </c>
-      <c r="O22" s="1" t="inlineStr"/>
-      <c r="P22" s="9" t="inlineStr">
-        <is>
-          <r>
-            <t xml:space="preserve">عاصم شيخو</t>
-          </r>
-        </is>
-      </c>
-      <c r="Q22" s="9" t="inlineStr"/>
-      <c r="R22" s="9" t="inlineStr"/>
-      <c r="S22" s="9" t="inlineStr"/>
-      <c r="T22" s="1" t="inlineStr"/>
-      <c r="U22" s="9" t="inlineStr">
-        <is>
-          <r>
-            <t xml:space="preserve">829983</t>
-          </r>
-        </is>
-      </c>
-      <c r="V22" s="9" t="inlineStr"/>
-      <c r="W22" s="1" t="inlineStr"/>
-      <c r="X22" s="10" t="inlineStr">
-        <is>
-          <r>
-            <t xml:space="preserve">51</t>
-          </r>
-        </is>
-      </c>
-      <c r="Y22" s="1" t="inlineStr"/>
-      <c r="Z22" s="1" t="inlineStr"/>
-    </row>
-    <row r="23" customHeight="1" ht="766">
-      <c r="A23" s="1" t="inlineStr"/>
-      <c r="B23" s="1" t="inlineStr"/>
-      <c r="C23" s="1" t="inlineStr"/>
-      <c r="D23" s="1" t="inlineStr"/>
-      <c r="E23" s="1" t="inlineStr"/>
-      <c r="F23" s="1" t="inlineStr"/>
-      <c r="G23" s="1" t="inlineStr"/>
-      <c r="H23" s="1" t="inlineStr"/>
-      <c r="I23" s="1" t="inlineStr"/>
-      <c r="J23" s="1" t="inlineStr"/>
-      <c r="K23" s="1" t="inlineStr"/>
-      <c r="L23" s="1" t="inlineStr"/>
-      <c r="M23" s="1" t="inlineStr"/>
-      <c r="N23" s="1" t="inlineStr"/>
-      <c r="O23" s="1" t="inlineStr"/>
-      <c r="P23" s="1" t="inlineStr"/>
-      <c r="Q23" s="1" t="inlineStr"/>
-      <c r="R23" s="1" t="inlineStr"/>
-      <c r="S23" s="1" t="inlineStr"/>
-      <c r="T23" s="1" t="inlineStr"/>
-      <c r="U23" s="1" t="inlineStr"/>
-      <c r="V23" s="1" t="inlineStr"/>
-      <c r="W23" s="1" t="inlineStr"/>
-      <c r="X23" s="1" t="inlineStr"/>
-      <c r="Y23" s="1" t="inlineStr"/>
-      <c r="Z23" s="1" t="inlineStr"/>
-    </row>
   </sheetData>
   <mergeCells>
     <mergeCell ref="B2:G4"/>
@@ -1180,10 +1088,6 @@
     <mergeCell ref="G20:L20"/>
     <mergeCell ref="P20:S20"/>
     <mergeCell ref="U20:V20"/>
-    <mergeCell ref="C22:E22"/>
-    <mergeCell ref="G22:L22"/>
-    <mergeCell ref="P22:S22"/>
-    <mergeCell ref="U22:V22"/>
   </mergeCells>
   <pageMargins left="0.0" right="0.0" top="0.0" bottom="0.00" header="0.0" footer="0.0"/>
   <pageSetup orientation="portrait"/>

</xml_diff>

<commit_message>
fix html supporting files invalid URL
</commit_message>
<xml_diff>
--- a/OfficeReport.xlsx
+++ b/OfficeReport.xlsx
@@ -237,7 +237,7 @@
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="412047054" name="Picture">
+        <xdr:cNvPr id="1367740448" name="Picture">
 </xdr:cNvPr>
         <xdr:cNvPicPr/>
       </xdr:nvPicPr>
@@ -522,7 +522,7 @@
       <c r="E8" s="5" t="inlineStr">
         <is>
           <r>
-            <t xml:space="preserve">2024-11-08T14:58:</t>
+            <t xml:space="preserve">2024-11-08T16:45:</t>
           </r>
         </is>
       </c>

</xml_diff>